<commit_message>
delete access to Pages/index, redirect to users/panel
</commit_message>
<xml_diff>
--- a/webroot/files/exemple_1.xlsx
+++ b/webroot/files/exemple_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="132" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="72" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Groupe</t>
   </si>
@@ -33,6 +33,15 @@
   </si>
   <si>
     <t>Jim Toast</t>
+  </si>
+  <si>
+    <t>Truc Much</t>
+  </si>
+  <si>
+    <t>Car Resse</t>
+  </si>
+  <si>
+    <t>Aloe Vera</t>
   </si>
 </sst>
 </file>
@@ -140,10 +149,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -167,7 +176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -184,6 +193,24 @@
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>